<commit_message>
Alteração estilo Login e adicionado User
</commit_message>
<xml_diff>
--- a/req_v4.xlsx
+++ b/req_v4.xlsx
@@ -1228,7 +1228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
@@ -2016,6 +2016,121 @@
         <v>32</v>
       </c>
       <c r="E34" t="inlineStr">
+        <is>
+          <t>cnc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>10/03/2022</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ifjeifje</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>32</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>cnc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>10/03/2022</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ifjeifje</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>32</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>cnc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>10/03/2022</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ifjeifje</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>32</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>cnc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>10/03/2022</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ifjeifje</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>32</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>cnc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>10/03/2022</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>ifjeifje</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>32</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>cnc2</t>
         </is>

</xml_diff>